<commit_message>
added parent item numbers
</commit_message>
<xml_diff>
--- a/data/rbEcoInfData.xlsx
+++ b/data/rbEcoInfData.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rblake\Documents\NCEAS\ecoInfoPaper\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9840" yWindow="0" windowWidth="25360" windowHeight="18780" tabRatio="500"/>
+    <workbookView xWindow="9840" yWindow="0" windowWidth="25365" windowHeight="18780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="59">
   <si>
     <t>Babcock</t>
   </si>
@@ -183,13 +188,19 @@
     <t>EVOSTC</t>
   </si>
   <si>
-    <t>Feder</t>
-  </si>
-  <si>
-    <t>Ferren</t>
-  </si>
-  <si>
-    <t>PWS Aquaculture Association</t>
+    <t>Parent Task</t>
+  </si>
+  <si>
+    <t>outside dates</t>
+  </si>
+  <si>
+    <t>can't find this</t>
+  </si>
+  <si>
+    <t>changed dates from 2003 to 2000</t>
+  </si>
+  <si>
+    <t>add project 813 to the spreadsheet</t>
   </si>
 </sst>
 </file>
@@ -233,6 +244,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -558,40 +577,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K31" sqref="A30:K31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.25" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1">
-        <v>1989</v>
-      </c>
-      <c r="H1">
-        <v>2000</v>
-      </c>
-      <c r="I1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
-        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -599,43 +603,49 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
+      <c r="E2">
+        <v>940</v>
+      </c>
       <c r="G2">
+        <v>1989</v>
+      </c>
+      <c r="H2">
+        <v>2000</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>974</v>
+      </c>
+      <c r="G3">
         <v>1993</v>
-      </c>
-      <c r="H2">
-        <v>2009</v>
-      </c>
-      <c r="I2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3">
-        <v>2000</v>
       </c>
       <c r="H3">
         <v>2009</v>
       </c>
       <c r="I3" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="K3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -643,22 +653,25 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>170</v>
       </c>
       <c r="G4">
-        <v>2002</v>
+        <v>2000</v>
       </c>
       <c r="H4">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="I4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="K4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -666,7 +679,10 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>170</v>
       </c>
       <c r="G5">
         <v>2002</v>
@@ -674,36 +690,39 @@
       <c r="H5">
         <v>2006</v>
       </c>
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
       <c r="K5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6">
+        <v>170</v>
+      </c>
+      <c r="G6">
+        <v>2002</v>
+      </c>
+      <c r="H6">
+        <v>2006</v>
+      </c>
+      <c r="K6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6">
-        <v>2011</v>
-      </c>
-      <c r="H6">
-        <v>2012</v>
-      </c>
-      <c r="I6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" t="s">
-        <v>17</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -712,42 +731,48 @@
         <v>11</v>
       </c>
       <c r="G7">
-        <v>2009</v>
+        <v>2011</v>
       </c>
       <c r="H7">
         <v>2012</v>
       </c>
       <c r="I7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="L7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G8">
-        <v>1989</v>
+        <v>2009</v>
       </c>
       <c r="H8">
-        <v>1989</v>
+        <v>2012</v>
       </c>
       <c r="I8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>16</v>
+      </c>
+      <c r="L8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -755,7 +780,10 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>645</v>
       </c>
       <c r="G9">
         <v>1989</v>
@@ -763,215 +791,245 @@
       <c r="H9">
         <v>1989</v>
       </c>
+      <c r="I9" t="s">
+        <v>20</v>
+      </c>
       <c r="K9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10">
+        <v>645</v>
+      </c>
+      <c r="G10">
+        <v>1989</v>
+      </c>
+      <c r="H10">
+        <v>1989</v>
+      </c>
+      <c r="K10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>23</v>
       </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10">
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>944</v>
+      </c>
+      <c r="G11">
         <v>1973</v>
       </c>
-      <c r="H10">
+      <c r="H11">
         <v>2010</v>
       </c>
-      <c r="I10" t="s">
-        <v>8</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="I11" t="s">
+        <v>8</v>
+      </c>
+      <c r="K11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
-      <c r="A11" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>24</v>
       </c>
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
         <v>22</v>
       </c>
-      <c r="G11">
-        <v>2003</v>
-      </c>
-      <c r="H11">
-        <v>2003</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="E12">
+        <v>742</v>
+      </c>
+      <c r="G12">
+        <v>2000</v>
+      </c>
+      <c r="H12">
+        <v>2000</v>
+      </c>
+      <c r="K12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" t="s">
+      <c r="L12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>25</v>
       </c>
-      <c r="B12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
         <v>26</v>
       </c>
-      <c r="G12">
-        <v>1993</v>
-      </c>
-      <c r="H12">
-        <v>2004</v>
-      </c>
-      <c r="I12" t="s">
-        <v>27</v>
-      </c>
-      <c r="K12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
+      <c r="E13">
+        <v>476</v>
       </c>
       <c r="G13">
         <v>1993</v>
       </c>
       <c r="H13">
+        <v>2004</v>
+      </c>
+      <c r="I13" t="s">
+        <v>27</v>
+      </c>
+      <c r="K13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14">
+        <v>279</v>
+      </c>
+      <c r="G14">
         <v>1993</v>
       </c>
-      <c r="I13" t="s">
+      <c r="H14">
+        <v>1993</v>
+      </c>
+      <c r="I14" t="s">
         <v>30</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
-      <c r="A14" t="s">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>32</v>
       </c>
-      <c r="B14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14">
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>1443</v>
+      </c>
+      <c r="G15">
         <v>2004</v>
       </c>
-      <c r="H14">
+      <c r="H15">
         <v>2008</v>
       </c>
-      <c r="I14" t="s">
-        <v>8</v>
-      </c>
-      <c r="K14" t="s">
+      <c r="I15" t="s">
+        <v>8</v>
+      </c>
+      <c r="K15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
-      <c r="A15" t="s">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>33</v>
       </c>
-      <c r="B15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15">
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>693</v>
+      </c>
+      <c r="G16">
         <v>1994</v>
       </c>
-      <c r="H15">
+      <c r="H16">
         <v>1997</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I16" t="s">
         <v>9</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
-      <c r="A16" t="s">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>34</v>
       </c>
-      <c r="B16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16">
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>413</v>
+      </c>
+      <c r="G17">
         <v>2003</v>
       </c>
-      <c r="H16">
+      <c r="H17">
         <v>2003</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I17" t="s">
         <v>35</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
-      <c r="A17" t="s">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>37</v>
       </c>
-      <c r="B17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G17">
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <v>532</v>
+      </c>
+      <c r="G18">
         <v>2004</v>
       </c>
-      <c r="H17">
+      <c r="H18">
         <v>2005</v>
       </c>
-      <c r="I17" t="s">
-        <v>8</v>
-      </c>
-      <c r="K17" t="s">
+      <c r="I18" t="s">
+        <v>8</v>
+      </c>
+      <c r="K18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
-      <c r="A18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G18">
-        <v>1997</v>
-      </c>
-      <c r="H18">
-        <v>2001</v>
-      </c>
-      <c r="I18" t="s">
-        <v>8</v>
-      </c>
-      <c r="K18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -979,7 +1037,10 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="E19">
+        <v>500</v>
       </c>
       <c r="G19">
         <v>1997</v>
@@ -988,13 +1049,13 @@
         <v>2001</v>
       </c>
       <c r="I19" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="K19" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1002,85 +1063,100 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>2</v>
+        <v>11</v>
+      </c>
+      <c r="E20">
+        <v>500</v>
       </c>
       <c r="G20">
-        <v>2004</v>
+        <v>1997</v>
       </c>
       <c r="H20">
-        <v>2004</v>
+        <v>2001</v>
       </c>
       <c r="I20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>718</v>
+      </c>
+      <c r="G21">
+        <v>2004</v>
+      </c>
+      <c r="H21">
+        <v>2004</v>
+      </c>
+      <c r="I21" t="s">
+        <v>41</v>
+      </c>
+      <c r="K21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>42</v>
       </c>
-      <c r="B21" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
         <v>22</v>
       </c>
-      <c r="G21">
+      <c r="E22">
+        <v>460</v>
+      </c>
+      <c r="G22">
         <v>1990</v>
       </c>
-      <c r="H21">
+      <c r="H22">
         <v>1995</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
-      <c r="A22" t="s">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>43</v>
       </c>
-      <c r="B22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>8</v>
-      </c>
-      <c r="G22">
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23">
+        <v>1408</v>
+      </c>
+      <c r="G23">
         <v>2001</v>
       </c>
-      <c r="H22">
+      <c r="H23">
         <v>2013</v>
       </c>
-      <c r="I22" t="s">
-        <v>8</v>
-      </c>
-      <c r="K22" t="s">
+      <c r="I23" t="s">
+        <v>8</v>
+      </c>
+      <c r="K23" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
-      <c r="A23" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23">
-        <v>1989</v>
-      </c>
-      <c r="H23">
-        <v>1998</v>
-      </c>
-      <c r="K23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -1088,22 +1164,22 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>22</v>
+      </c>
+      <c r="E24">
+        <v>565</v>
       </c>
       <c r="G24">
-        <v>1986</v>
+        <v>1989</v>
       </c>
       <c r="H24">
-        <v>1996</v>
-      </c>
-      <c r="I24" t="s">
-        <v>8</v>
+        <v>1998</v>
       </c>
       <c r="K24" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -1113,68 +1189,80 @@
       <c r="D25" t="s">
         <v>8</v>
       </c>
+      <c r="E25">
+        <v>565</v>
+      </c>
       <c r="G25">
-        <v>1984</v>
+        <v>1986</v>
       </c>
       <c r="H25">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="I25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K25" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26">
+        <v>565</v>
+      </c>
+      <c r="G26">
+        <v>1984</v>
+      </c>
+      <c r="H26">
+        <v>1998</v>
+      </c>
+      <c r="I26" t="s">
+        <v>9</v>
+      </c>
+      <c r="K26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>46</v>
       </c>
-      <c r="B26" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
         <v>11</v>
       </c>
-      <c r="G26">
+      <c r="E27">
+        <v>814</v>
+      </c>
+      <c r="G27">
         <v>2000</v>
       </c>
-      <c r="H26">
+      <c r="H27">
         <v>2009</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I27" t="s">
         <v>47</v>
       </c>
-      <c r="K26" t="s">
+      <c r="K27" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="A27" t="s">
+      <c r="L27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>49</v>
-      </c>
-      <c r="B27" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G27">
-        <v>1993</v>
-      </c>
-      <c r="H27">
-        <v>2004</v>
-      </c>
-      <c r="I27" t="s">
-        <v>50</v>
-      </c>
-      <c r="K27" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="A28" t="s">
-        <v>51</v>
       </c>
       <c r="B28" t="s">
         <v>1</v>
@@ -1182,60 +1270,46 @@
       <c r="D28" t="s">
         <v>26</v>
       </c>
+      <c r="E28">
+        <v>476</v>
+      </c>
       <c r="G28">
+        <v>1993</v>
+      </c>
+      <c r="H28">
+        <v>2004</v>
+      </c>
+      <c r="I28" t="s">
+        <v>50</v>
+      </c>
+      <c r="K28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29">
+        <v>1002</v>
+      </c>
+      <c r="G29">
         <v>1998</v>
       </c>
-      <c r="H28">
+      <c r="H29">
         <v>1999</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I29" t="s">
         <v>52</v>
       </c>
-      <c r="K28" t="s">
+      <c r="K29" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
-      <c r="A29" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" t="s">
-        <v>2</v>
-      </c>
-      <c r="G29">
-        <v>1989</v>
-      </c>
-      <c r="H29">
-        <v>1991</v>
-      </c>
-      <c r="I29" t="s">
-        <v>41</v>
-      </c>
-      <c r="K29" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="A30" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" t="s">
-        <v>22</v>
-      </c>
-      <c r="G30">
-        <v>1994</v>
-      </c>
-      <c r="H30">
-        <v>1997</v>
-      </c>
-      <c r="K30" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>